<commit_message>
Bouton retour à l'étape de validation
</commit_message>
<xml_diff>
--- a/productList_xlsx/productsList.xlsx
+++ b/productList_xlsx/productsList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\Ti-Lichous\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\Ti-Lichous\productList_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1030E27-75ED-42C8-A4EF-2E6E1D52F539}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778FC48F-57C8-4342-B62D-4C1AF3A09F07}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{CA837B9F-5D09-41D1-AF09-D7DD8EB744DB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Lichouseries</t>
   </si>
@@ -39,19 +39,91 @@
     <t>Pause Gourmande Apéritive</t>
   </si>
   <si>
-    <t>Café, thé, jus de pommes ou raisins.Triskels au chocolat.Meringues</t>
-  </si>
-  <si>
-    <t>Café, thé, jus de pommes ou raisins.Gâteau breton.Triskels au chocolat</t>
-  </si>
-  <si>
-    <t>Café, thé, jus de pommes ou raisins.Gâteau breton.Triskels au chocolat.Crêpes roulées</t>
-  </si>
-  <si>
-    <t>Cidre, vin blanc, jus de pommes.Assortiment de crêpes roulées salées</t>
-  </si>
-  <si>
-    <t>Cidre, vin blanc, jus de raisins.Assortiment de lichouseries sucrées et salées</t>
+    <t>Petit choux de blé noir garni</t>
+  </si>
+  <si>
+    <t>Blini garni</t>
+  </si>
+  <si>
+    <t>Mini-roulées de blé noir</t>
+  </si>
+  <si>
+    <t>Tuiles</t>
+  </si>
+  <si>
+    <t>Triskels au chocolat</t>
+  </si>
+  <si>
+    <t>Truffes</t>
+  </si>
+  <si>
+    <t>Meringues</t>
+  </si>
+  <si>
+    <t>Kig ha farz</t>
+  </si>
+  <si>
+    <t>Potée de pouldrezic (aux choux)</t>
+  </si>
+  <si>
+    <t>Potée Guérandaise (fèves, lard, saucisses)</t>
+  </si>
+  <si>
+    <t>Frigousse de bœuf</t>
+  </si>
+  <si>
+    <t>Cotriade ou matelote</t>
+  </si>
+  <si>
+    <t>Poulet au cidre</t>
+  </si>
+  <si>
+    <t>Jambon à l'os (environ 30 pers.)</t>
+  </si>
+  <si>
+    <t>Buffet de crêpes : peut-être accompagné de garnitures (sucre, confitures, ...)</t>
+  </si>
+  <si>
+    <t>1 galette blé noir_2 crêpes froment</t>
+  </si>
+  <si>
+    <t>Café, thé, jus de pommes ou raisins_Triskels au chocolat_Meringues</t>
+  </si>
+  <si>
+    <t>Café, thé, jus de pommes ou raisins_Gâteau breton_Triskels au chocolat</t>
+  </si>
+  <si>
+    <t>Café, thé, jus de pommes ou raisins_Gâteau breton_Triskels au chocolat_Crêpes roulées</t>
+  </si>
+  <si>
+    <t>Cidre, vin blanc, jus de pommes_Assortiment de crêpes roulées salées</t>
+  </si>
+  <si>
+    <t>Cidre, vin blanc, jus de raisins_Assortiment de lichouseries sucrées et salées</t>
+  </si>
+  <si>
+    <t>2 galette blé noir_2 crêpes froment</t>
+  </si>
+  <si>
+    <t>galettes blé noir à volonté_crêpes froment à volonté</t>
+  </si>
+  <si>
+    <t>1 galette blé noir_1 crêpes froment</t>
+  </si>
+  <si>
+    <t>Assortiment de lichouseries_2 galettes blé noir_Salade_2 crêpes froment</t>
+  </si>
+  <si>
+    <t>Cidre artisanal Kerné</t>
+  </si>
+  <si>
+    <t>Cidre fermier Melenig</t>
+  </si>
+  <si>
+    <t>Cidre Kerné</t>
+  </si>
+  <si>
+    <t>Jus de pomme Kerné</t>
   </si>
 </sst>
 </file>
@@ -426,7 +498,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,104 +521,152 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C2" s="4" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>

</xml_diff>

<commit_message>
Enregistrement des articles dans le tableau pour les particuliers
</commit_message>
<xml_diff>
--- a/productList_xlsx/productsList.xlsx
+++ b/productList_xlsx/productsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\Ti-Lichous\productList_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778FC48F-57C8-4342-B62D-4C1AF3A09F07}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81512C78-9F5E-4CF6-AF5F-EE56776FA038}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{CA837B9F-5D09-41D1-AF09-D7DD8EB744DB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Lichouseries</t>
   </si>
@@ -112,18 +112,6 @@
   </si>
   <si>
     <t>Assortiment de lichouseries_2 galettes blé noir_Salade_2 crêpes froment</t>
-  </si>
-  <si>
-    <t>Cidre artisanal Kerné</t>
-  </si>
-  <si>
-    <t>Cidre fermier Melenig</t>
-  </si>
-  <si>
-    <t>Cidre Kerné</t>
-  </si>
-  <si>
-    <t>Jus de pomme Kerné</t>
   </si>
 </sst>
 </file>
@@ -498,7 +486,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,9 +572,7 @@
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
@@ -594,9 +580,7 @@
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
@@ -604,9 +588,7 @@
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
@@ -614,9 +596,7 @@
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>

</xml_diff>

<commit_message>
Récupération des produits sélectionnés
</commit_message>
<xml_diff>
--- a/productList_xlsx/productsList.xlsx
+++ b/productList_xlsx/productsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\Ti-Lichous\productList_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81512C78-9F5E-4CF6-AF5F-EE56776FA038}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7EA560-06F3-4BEA-8DDF-CB0060D287DC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{CA837B9F-5D09-41D1-AF09-D7DD8EB744DB}"/>
   </bookViews>
@@ -105,13 +105,13 @@
     <t>2 galette blé noir_2 crêpes froment</t>
   </si>
   <si>
-    <t>galettes blé noir à volonté_crêpes froment à volonté</t>
-  </si>
-  <si>
     <t>1 galette blé noir_1 crêpes froment</t>
   </si>
   <si>
     <t>Assortiment de lichouseries_2 galettes blé noir_Salade_2 crêpes froment</t>
+  </si>
+  <si>
+    <t>Galettes blé noir à volonté_crêpes froment à volonté</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +541,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>22</v>
@@ -553,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -563,7 +563,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>

</xml_diff>